<commit_message>
se suben archivos modificados
se modifican archivos para realizar correcciones del tutor
</commit_message>
<xml_diff>
--- a/Diagrama-Márquez.xlsx
+++ b/Diagrama-Márquez.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="104">
   <si>
     <t>Tabla</t>
   </si>
@@ -82,6 +82,12 @@
     <t>id sobre que tipo de cliente es</t>
   </si>
   <si>
+    <t>country_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id de cada país </t>
+  </si>
+  <si>
     <t>mail</t>
   </si>
   <si>
@@ -115,10 +121,25 @@
     <t>id primario de cada region</t>
   </si>
   <si>
-    <t>country_id</t>
+    <t>id país de la venta</t>
   </si>
   <si>
-    <t>id país de la venta</t>
+    <t>postal_code_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id codigo postal de la region </t>
+  </si>
+  <si>
+    <t>city_id</t>
+  </si>
+  <si>
+    <t>id sobre la ciudad de la venta</t>
+  </si>
+  <si>
+    <t>state_id</t>
+  </si>
+  <si>
+    <t>id del estado donde se realizo la venta</t>
   </si>
   <si>
     <t>region dentro de los Estados Unidos</t>
@@ -130,13 +151,7 @@
     <t>TABLA DIMENSIONAL DONDE SE GUARDAN LOS DATOS DE LOS CODIGOS POSTALES</t>
   </si>
   <si>
-    <t>postal_code_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id codigo postal de la region </t>
-  </si>
-  <si>
-    <t>id de cada region</t>
+    <t xml:space="preserve">id primario del codigo postal de la region </t>
   </si>
   <si>
     <t xml:space="preserve">codigo postal de la region </t>
@@ -151,9 +166,6 @@
     <t xml:space="preserve">id primario de cada país </t>
   </si>
   <si>
-    <t>id de cada cliente</t>
-  </si>
-  <si>
     <t>país de la venta</t>
   </si>
   <si>
@@ -163,10 +175,7 @@
     <t>TABLA DIMENSIONAL DONDE SE GUARDAN LOS DATOS SOBRE LA CIUDAD DONDE SE REALIZO LA VENTA</t>
   </si>
   <si>
-    <t>city_id</t>
-  </si>
-  <si>
-    <t>id ciudad de la venta</t>
+    <t>id primario sobre la ciudad de la venta</t>
   </si>
   <si>
     <t>ciudad de la venta</t>
@@ -178,10 +187,7 @@
     <t>TABLA DIMENSIONAL DONDE SE GUARDAN LOS DATOS SOBRE EL ESTADO DONDE SE REALIZO LA VENTA</t>
   </si>
   <si>
-    <t>state_id</t>
-  </si>
-  <si>
-    <t>id estado donde se realizo la venta</t>
+    <t>id primario del estado donde se realizo la venta</t>
   </si>
   <si>
     <t>estado donde se realizo la venta</t>
@@ -197,6 +203,9 @@
   </si>
   <si>
     <t>ditail_id</t>
+  </si>
+  <si>
+    <t>id de cada cliente</t>
   </si>
   <si>
     <t>order_date</t>
@@ -386,14 +395,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFF3F3F3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -465,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -505,15 +514,10 @@
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="5" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="6" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -522,8 +526,9 @@
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="6" fillId="5" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -652,7 +657,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B5:I9" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B5:I10" displayName="Table_1" id="1">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -764,7 +769,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B14:I16" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B15:I17" displayName="Table_2" id="2">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -780,7 +785,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B21:I24" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B22:I28" displayName="Table_3" id="3">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -796,7 +801,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B29:I32" displayName="Table_4" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B33:I35" displayName="Table_4" id="4">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -812,7 +817,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B37:I40" displayName="Table_5" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B40:I42" displayName="Table_5" id="5">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -828,7 +833,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B45:I48" displayName="Table_6" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B47:I49" displayName="Table_6" id="6">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -844,7 +849,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B53:I56" displayName="Table_7" id="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B54:I56" displayName="Table_7" id="7">
   <tableColumns count="8">
     <tableColumn name="KEY" id="1"/>
     <tableColumn name="COLUMN" id="2"/>
@@ -1406,18 +1411,20 @@
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="8">
-        <v>40.0</v>
-      </c>
-      <c r="F9" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="G9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>15</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1447,14 +1454,28 @@
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1503,18 +1524,14 @@
     </row>
     <row r="12" ht="17.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1536,10 +1553,10 @@
     <row r="13" ht="17.25" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1567,30 +1584,18 @@
     </row>
     <row r="14" ht="17.25" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1611,29 +1616,29 @@
     </row>
     <row r="15" ht="17.25" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="B15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>28</v>
+      <c r="G15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1656,16 +1661,16 @@
     <row r="16" ht="17.25" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="8">
-        <v>40.0</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>8</v>
@@ -1674,10 +1679,10 @@
         <v>15</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1699,14 +1704,30 @@
     </row>
     <row r="17" ht="17.25" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="B17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1755,18 +1776,14 @@
     </row>
     <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1788,10 +1805,10 @@
     <row r="20" ht="17.25" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1819,30 +1836,18 @@
     </row>
     <row r="21" ht="17.25" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1863,29 +1868,29 @@
     </row>
     <row r="22" ht="17.25" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="B22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>33</v>
+      <c r="G22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1908,7 +1913,7 @@
     <row r="23" ht="17.25" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>34</v>
@@ -1952,21 +1957,23 @@
     <row r="24" ht="17.25" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="8">
-        <v>40.0</v>
-      </c>
       <c r="F24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="9"/>
       <c r="H24" s="8" t="s">
         <v>15</v>
       </c>
@@ -1993,14 +2000,30 @@
     </row>
     <row r="25" ht="17.25" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="B25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2021,14 +2044,30 @@
     </row>
     <row r="26" ht="17.25" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="B26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2048,183 +2087,161 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" ht="17.25" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
     </row>
     <row r="28" ht="17.25" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
     </row>
     <row r="29" ht="17.25" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="13"/>
-      <c r="V29" s="13"/>
-      <c r="W29" s="13"/>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13"/>
-      <c r="Z29" s="13"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13"/>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" ht="17.25" customHeight="1">
       <c r="A31" s="10"/>
-      <c r="B31" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>41</v>
-      </c>
+      <c r="B31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -2245,30 +2262,18 @@
     </row>
     <row r="32" ht="17.25" customHeight="1">
       <c r="A32" s="10"/>
-      <c r="B32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="B32" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
@@ -2288,75 +2293,119 @@
       <c r="Z32" s="13"/>
     </row>
     <row r="33" ht="17.25" customHeight="1">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
     </row>
     <row r="34" ht="17.25" customHeight="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="13"/>
     </row>
     <row r="35" ht="17.25" customHeight="1">
       <c r="A35" s="10"/>
-      <c r="B35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="6"/>
+      <c r="B35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2376,107 +2425,75 @@
       <c r="Z35" s="13"/>
     </row>
     <row r="36" ht="17.25" customHeight="1">
-      <c r="A36" s="10"/>
-      <c r="B36" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
     </row>
     <row r="37" ht="17.25" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
-      <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
-      <c r="W37" s="13"/>
-      <c r="X37" s="13"/>
-      <c r="Y37" s="13"/>
-      <c r="Z37" s="13"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
     </row>
     <row r="38" ht="17.25" customHeight="1">
       <c r="A38" s="10"/>
-      <c r="B38" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="B38" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="6"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
@@ -2497,30 +2514,18 @@
     </row>
     <row r="39" ht="17.25" customHeight="1">
       <c r="A39" s="10"/>
-      <c r="B39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="B39" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="17"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -2541,23 +2546,29 @@
     </row>
     <row r="40" ht="17.25" customHeight="1">
       <c r="A40" s="10"/>
-      <c r="B40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="8">
-        <v>40.0</v>
-      </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="8" t="s">
-        <v>47</v>
+      <c r="B40" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
@@ -2578,75 +2589,97 @@
       <c r="Z40" s="13"/>
     </row>
     <row r="41" ht="17.25" customHeight="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-      <c r="X41" s="1"/>
-      <c r="Y41" s="1"/>
-      <c r="Z41" s="1"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
     </row>
     <row r="42" ht="17.25" customHeight="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="1"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
     </row>
     <row r="43" ht="17.25" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="6"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2667,18 +2700,14 @@
     </row>
     <row r="44" ht="17.25" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="17"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2699,30 +2728,18 @@
     </row>
     <row r="45" ht="17.25" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I45" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="B45" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="6"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2743,30 +2760,18 @@
     </row>
     <row r="46" ht="17.25" customHeight="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="B46" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2787,29 +2792,29 @@
     </row>
     <row r="47" ht="17.25" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="8" t="s">
+      <c r="B47" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>41</v>
+      <c r="G47" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2832,28 +2837,28 @@
     <row r="48" ht="17.25" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="8">
-        <v>40.0</v>
-      </c>
       <c r="F48" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -2875,14 +2880,30 @@
     </row>
     <row r="49" ht="17.25" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="B49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2931,18 +2952,14 @@
     </row>
     <row r="51" ht="17.25" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="6"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2963,18 +2980,18 @@
     </row>
     <row r="52" ht="17.25" customHeight="1">
       <c r="A52" s="1"/>
-      <c r="B52" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="17"/>
+      <c r="B52" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="6"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2995,30 +3012,18 @@
     </row>
     <row r="53" ht="17.25" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I53" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="B53" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="17"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -3039,29 +3044,29 @@
     </row>
     <row r="54" ht="17.25" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" s="8" t="s">
+      <c r="B54" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>56</v>
+      <c r="G54" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -3084,10 +3089,10 @@
     <row r="55" ht="17.25" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>14</v>
@@ -3102,10 +3107,10 @@
         <v>15</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -3131,10 +3136,10 @@
         <v>15</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E56" s="8">
         <v>40.0</v>
@@ -3149,7 +3154,7 @@
         <v>15</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -3231,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -3263,7 +3268,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -3357,7 +3362,7 @@
         <v>16</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -3383,7 +3388,7 @@
         <v>18</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>14</v>
@@ -3401,7 +3406,7 @@
         <v>15</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -3427,10 +3432,10 @@
         <v>15</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>15</v>
@@ -3445,7 +3450,7 @@
         <v>15</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -3471,13 +3476,13 @@
         <v>15</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>15</v>
@@ -3489,7 +3494,7 @@
         <v>15</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -3515,13 +3520,13 @@
         <v>15</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>15</v>
@@ -3533,7 +3538,7 @@
         <v>15</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -3559,13 +3564,13 @@
         <v>15</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>15</v>
@@ -3577,7 +3582,7 @@
         <v>15</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -3659,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -3691,7 +3696,7 @@
         <v>2</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -3767,7 +3772,7 @@
         <v>12</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>14</v>
@@ -3785,7 +3790,7 @@
         <v>16</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3811,7 +3816,7 @@
         <v>18</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>14</v>
@@ -3829,7 +3834,7 @@
         <v>15</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -3855,10 +3860,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E75" s="8">
         <v>100.0</v>
@@ -3873,7 +3878,7 @@
         <v>15</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -3955,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
@@ -3987,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
@@ -4063,7 +4068,7 @@
         <v>12</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>14</v>
@@ -4081,7 +4086,7 @@
         <v>16</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -4107,7 +4112,7 @@
         <v>18</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>14</v>
@@ -4125,7 +4130,7 @@
         <v>15</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -4151,10 +4156,10 @@
         <v>15</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E83" s="8">
         <v>40.0</v>
@@ -4169,7 +4174,7 @@
         <v>15</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -4251,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -4283,7 +4288,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -4359,7 +4364,7 @@
         <v>12</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>14</v>
@@ -4377,7 +4382,7 @@
         <v>16</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
@@ -4403,7 +4408,7 @@
         <v>18</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>14</v>
@@ -4421,7 +4426,7 @@
         <v>15</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -4447,10 +4452,10 @@
         <v>15</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E91" s="8">
         <v>40.0</v>
@@ -4465,7 +4470,7 @@
         <v>15</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
@@ -4547,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -4579,7 +4584,7 @@
         <v>2</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D95" s="16"/>
       <c r="E95" s="16"/>
@@ -4651,29 +4656,29 @@
     </row>
     <row r="97" ht="17.25" customHeight="1">
       <c r="A97" s="10"/>
-      <c r="B97" s="24" t="s">
+      <c r="B97" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D97" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D97" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E97" s="25" t="s">
+      <c r="E97" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F97" s="24" t="s">
+      <c r="F97" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G97" s="25" t="s">
+      <c r="G97" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H97" s="24" t="s">
+      <c r="H97" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I97" s="25" t="s">
-        <v>94</v>
+      <c r="I97" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="J97" s="13"/>
       <c r="K97" s="13"/>
@@ -4699,7 +4704,7 @@
         <v>18</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>14</v>
@@ -4717,7 +4722,7 @@
         <v>15</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J98" s="13"/>
       <c r="K98" s="13"/>
@@ -4743,10 +4748,10 @@
         <v>15</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E99" s="8">
         <v>40.0</v>
@@ -4761,7 +4766,7 @@
         <v>15</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J99" s="13"/>
       <c r="K99" s="13"/>
@@ -4843,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
@@ -4875,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
@@ -4951,7 +4956,7 @@
         <v>12</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>14</v>
@@ -4969,7 +4974,7 @@
         <v>16</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
@@ -4995,7 +5000,7 @@
         <v>15</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>14</v>
@@ -5013,7 +5018,7 @@
         <v>15</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
@@ -5091,10 +5096,10 @@
     </row>
     <row r="109" ht="17.25" customHeight="1">
       <c r="A109" s="1"/>
-      <c r="B109" s="22" t="s">
+      <c r="B109" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C109" s="26"/>
+      <c r="C109" s="23"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
@@ -5121,10 +5126,10 @@
     </row>
     <row r="110" ht="17.25" customHeight="1">
       <c r="A110" s="1"/>
-      <c r="B110" s="22" t="s">
+      <c r="B110" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C110" s="27"/>
+      <c r="C110" s="24"/>
       <c r="D110" s="16"/>
       <c r="E110" s="16"/>
       <c r="F110" s="16"/>
@@ -5151,7 +5156,7 @@
     </row>
     <row r="111" ht="17.25" customHeight="1">
       <c r="A111" s="1"/>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C111" s="18" t="s">
@@ -5195,14 +5200,14 @@
     </row>
     <row r="112" ht="17.25" customHeight="1">
       <c r="A112" s="1"/>
-      <c r="B112" s="28"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
-      <c r="F112" s="24"/>
-      <c r="G112" s="24"/>
-      <c r="H112" s="24"/>
-      <c r="I112" s="24"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
@@ -5223,14 +5228,14 @@
     </row>
     <row r="113" ht="17.25" customHeight="1">
       <c r="A113" s="1"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
+      <c r="B113" s="26"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
@@ -5251,14 +5256,14 @@
     </row>
     <row r="114" ht="17.25" customHeight="1">
       <c r="A114" s="1"/>
-      <c r="B114" s="28"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="24"/>
-      <c r="G114" s="24"/>
-      <c r="H114" s="24"/>
-      <c r="I114" s="24"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="21"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
@@ -5279,14 +5284,14 @@
     </row>
     <row r="115" ht="17.25" customHeight="1">
       <c r="A115" s="1"/>
-      <c r="B115" s="19"/>
-      <c r="C115" s="29"/>
-      <c r="D115" s="29"/>
-      <c r="E115" s="29"/>
-      <c r="F115" s="29"/>
-      <c r="G115" s="29"/>
-      <c r="H115" s="29"/>
-      <c r="I115" s="29"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="27"/>
+      <c r="I115" s="27"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
@@ -5307,14 +5312,14 @@
     </row>
     <row r="116" ht="17.25" customHeight="1">
       <c r="A116" s="1"/>
-      <c r="B116" s="28"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
-      <c r="G116" s="24"/>
-      <c r="H116" s="24"/>
-      <c r="I116" s="24"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="21"/>
+      <c r="H116" s="21"/>
+      <c r="I116" s="21"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
@@ -5335,14 +5340,14 @@
     </row>
     <row r="117" ht="17.25" customHeight="1">
       <c r="A117" s="1"/>
-      <c r="B117" s="19"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="27"/>
+      <c r="G117" s="27"/>
+      <c r="H117" s="27"/>
+      <c r="I117" s="27"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
@@ -5363,14 +5368,14 @@
     </row>
     <row r="118" ht="17.25" customHeight="1">
       <c r="A118" s="1"/>
-      <c r="B118" s="28"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="24"/>
-      <c r="F118" s="24"/>
-      <c r="G118" s="24"/>
-      <c r="H118" s="24"/>
-      <c r="I118" s="24"/>
+      <c r="B118" s="25"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="21"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="21"/>
+      <c r="G118" s="21"/>
+      <c r="H118" s="21"/>
+      <c r="I118" s="21"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
@@ -5391,14 +5396,14 @@
     </row>
     <row r="119" ht="17.25" customHeight="1">
       <c r="A119" s="1"/>
-      <c r="B119" s="19"/>
-      <c r="C119" s="29"/>
-      <c r="D119" s="29"/>
-      <c r="E119" s="29"/>
-      <c r="F119" s="29"/>
-      <c r="G119" s="29"/>
-      <c r="H119" s="29"/>
-      <c r="I119" s="29"/>
+      <c r="B119" s="26"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="27"/>
+      <c r="H119" s="27"/>
+      <c r="I119" s="27"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
@@ -5419,14 +5424,14 @@
     </row>
     <row r="120" ht="17.25" customHeight="1">
       <c r="A120" s="1"/>
-      <c r="B120" s="28"/>
-      <c r="C120" s="24"/>
-      <c r="D120" s="24"/>
-      <c r="E120" s="24"/>
-      <c r="F120" s="24"/>
-      <c r="G120" s="24"/>
-      <c r="H120" s="24"/>
-      <c r="I120" s="24"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="21"/>
+      <c r="E120" s="21"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="21"/>
+      <c r="H120" s="21"/>
+      <c r="I120" s="21"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
@@ -5503,10 +5508,10 @@
     </row>
     <row r="123" ht="17.25" customHeight="1">
       <c r="A123" s="1"/>
-      <c r="B123" s="22" t="s">
+      <c r="B123" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C123" s="26"/>
+      <c r="C123" s="23"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -5533,10 +5538,10 @@
     </row>
     <row r="124" ht="17.25" customHeight="1">
       <c r="A124" s="1"/>
-      <c r="B124" s="22" t="s">
+      <c r="B124" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C124" s="27"/>
+      <c r="C124" s="24"/>
       <c r="D124" s="16"/>
       <c r="E124" s="16"/>
       <c r="F124" s="16"/>
@@ -5563,7 +5568,7 @@
     </row>
     <row r="125" ht="17.25" customHeight="1">
       <c r="A125" s="1"/>
-      <c r="B125" s="23" t="s">
+      <c r="B125" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C125" s="18" t="s">
@@ -5607,14 +5612,14 @@
     </row>
     <row r="126" ht="17.25" customHeight="1">
       <c r="A126" s="1"/>
-      <c r="B126" s="28"/>
-      <c r="C126" s="24"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="24"/>
-      <c r="F126" s="24"/>
-      <c r="G126" s="24"/>
-      <c r="H126" s="24"/>
-      <c r="I126" s="24"/>
+      <c r="B126" s="25"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="21"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
@@ -5635,14 +5640,14 @@
     </row>
     <row r="127" ht="17.25" customHeight="1">
       <c r="A127" s="1"/>
-      <c r="B127" s="19"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="29"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="29"/>
-      <c r="G127" s="29"/>
-      <c r="H127" s="29"/>
-      <c r="I127" s="29"/>
+      <c r="B127" s="26"/>
+      <c r="C127" s="27"/>
+      <c r="D127" s="27"/>
+      <c r="E127" s="27"/>
+      <c r="F127" s="27"/>
+      <c r="G127" s="27"/>
+      <c r="H127" s="27"/>
+      <c r="I127" s="27"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
@@ -5663,14 +5668,14 @@
     </row>
     <row r="128" ht="17.25" customHeight="1">
       <c r="A128" s="1"/>
-      <c r="B128" s="28"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="24"/>
-      <c r="E128" s="24"/>
-      <c r="F128" s="24"/>
-      <c r="G128" s="24"/>
-      <c r="H128" s="24"/>
-      <c r="I128" s="24"/>
+      <c r="B128" s="25"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="21"/>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+      <c r="I128" s="21"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
@@ -5691,14 +5696,14 @@
     </row>
     <row r="129" ht="17.25" customHeight="1">
       <c r="A129" s="1"/>
-      <c r="B129" s="19"/>
-      <c r="C129" s="29"/>
-      <c r="D129" s="29"/>
-      <c r="E129" s="29"/>
-      <c r="F129" s="29"/>
-      <c r="G129" s="29"/>
-      <c r="H129" s="29"/>
-      <c r="I129" s="29"/>
+      <c r="B129" s="26"/>
+      <c r="C129" s="27"/>
+      <c r="D129" s="27"/>
+      <c r="E129" s="27"/>
+      <c r="F129" s="27"/>
+      <c r="G129" s="27"/>
+      <c r="H129" s="27"/>
+      <c r="I129" s="27"/>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
@@ -5719,14 +5724,14 @@
     </row>
     <row r="130" ht="17.25" customHeight="1">
       <c r="A130" s="1"/>
-      <c r="B130" s="28"/>
-      <c r="C130" s="24"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="24"/>
-      <c r="F130" s="24"/>
-      <c r="G130" s="24"/>
-      <c r="H130" s="24"/>
-      <c r="I130" s="24"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="21"/>
+      <c r="E130" s="21"/>
+      <c r="F130" s="21"/>
+      <c r="G130" s="21"/>
+      <c r="H130" s="21"/>
+      <c r="I130" s="21"/>
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
@@ -5747,14 +5752,14 @@
     </row>
     <row r="131" ht="17.25" customHeight="1">
       <c r="A131" s="1"/>
-      <c r="B131" s="19"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="29"/>
-      <c r="E131" s="29"/>
-      <c r="F131" s="29"/>
-      <c r="G131" s="29"/>
-      <c r="H131" s="29"/>
-      <c r="I131" s="29"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="27"/>
+      <c r="D131" s="27"/>
+      <c r="E131" s="27"/>
+      <c r="F131" s="27"/>
+      <c r="G131" s="27"/>
+      <c r="H131" s="27"/>
+      <c r="I131" s="27"/>
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
@@ -5775,14 +5780,14 @@
     </row>
     <row r="132" ht="17.25" customHeight="1">
       <c r="A132" s="1"/>
-      <c r="B132" s="28"/>
-      <c r="C132" s="24"/>
-      <c r="D132" s="24"/>
-      <c r="E132" s="24"/>
-      <c r="F132" s="24"/>
-      <c r="G132" s="24"/>
-      <c r="H132" s="24"/>
-      <c r="I132" s="24"/>
+      <c r="B132" s="25"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="21"/>
+      <c r="E132" s="21"/>
+      <c r="F132" s="21"/>
+      <c r="G132" s="21"/>
+      <c r="H132" s="21"/>
+      <c r="I132" s="21"/>
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
@@ -5803,14 +5808,14 @@
     </row>
     <row r="133" ht="17.25" customHeight="1">
       <c r="A133" s="1"/>
-      <c r="B133" s="19"/>
-      <c r="C133" s="29"/>
-      <c r="D133" s="29"/>
-      <c r="E133" s="29"/>
-      <c r="F133" s="29"/>
-      <c r="G133" s="29"/>
-      <c r="H133" s="29"/>
-      <c r="I133" s="29"/>
+      <c r="B133" s="26"/>
+      <c r="C133" s="27"/>
+      <c r="D133" s="27"/>
+      <c r="E133" s="27"/>
+      <c r="F133" s="27"/>
+      <c r="G133" s="27"/>
+      <c r="H133" s="27"/>
+      <c r="I133" s="27"/>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
@@ -5831,14 +5836,14 @@
     </row>
     <row r="134" ht="17.25" customHeight="1">
       <c r="A134" s="1"/>
-      <c r="B134" s="28"/>
-      <c r="C134" s="24"/>
-      <c r="D134" s="24"/>
-      <c r="E134" s="24"/>
-      <c r="F134" s="24"/>
-      <c r="G134" s="24"/>
-      <c r="H134" s="24"/>
-      <c r="I134" s="24"/>
+      <c r="B134" s="25"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="21"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="21"/>
+      <c r="H134" s="21"/>
+      <c r="I134" s="21"/>
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
@@ -28065,18 +28070,18 @@
   <mergeCells count="30">
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C12:I12"/>
     <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C14:I14"/>
     <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C46:I46"/>
     <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C53:I53"/>
     <mergeCell ref="C59:I59"/>
     <mergeCell ref="C60:I60"/>
     <mergeCell ref="C70:I70"/>

</xml_diff>